<commit_message>
Added Testing tools and diagnostic test data
</commit_message>
<xml_diff>
--- a/Simulation/CSARCH2 Proj Diagnostics.xlsx
+++ b/Simulation/CSARCH2 Proj Diagnostics.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Miguel Escalona\Github\CSARCH2_Project\Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1252CEE2-4BBD-4680-9A61-06462AB8D134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6969BB-A2A5-4D22-8F34-026A1BB24160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E5B5E468-C3F2-49F0-9D6C-48D86FBE0D23}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{E5B5E468-C3F2-49F0-9D6C-48D86FBE0D23}"/>
   </bookViews>
   <sheets>
     <sheet name="Unicode.java Peformance Test" sheetId="2" r:id="rId1"/>
     <sheet name="70 Run" sheetId="5" r:id="rId2"/>
     <sheet name="Main_Sheet" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
+    <sheet name="70 Run Sheet" sheetId="4" r:id="rId4"/>
+    <sheet name="Raw" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Hex</t>
   </si>
@@ -66,12 +66,21 @@
   <si>
     <t>New Implementation</t>
   </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>2c92a24</t>
+  </si>
+  <si>
+    <t>Concatenated</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +90,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -108,19 +125,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -162,6 +222,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1091,7 +1154,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1105,11 +1168,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-PH"/>
-              <a:t>Unicode.java</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-PH" baseline="0"/>
-              <a:t> 70 Runs Performance Test</a:t>
+              <a:t>Unicode.java 70 Runs Performance Test</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1127,7 +1186,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1154,7 +1213,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$B$1</c:f>
+              <c:f>'70 Run Sheet'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1189,7 +1248,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1246,7 +1305,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$B$2:$B$17</c:f>
+              <c:f>'70 Run Sheet'!$B$2:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1313,7 +1372,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$C$1</c:f>
+              <c:f>'70 Run Sheet'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1348,7 +1407,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1405,7 +1464,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$C$2:$C$17</c:f>
+              <c:f>'70 Run Sheet'!$C$2:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1472,7 +1531,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$D$1</c:f>
+              <c:f>'70 Run Sheet'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1507,7 +1566,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1564,7 +1623,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$D$2:$D$17</c:f>
+              <c:f>'70 Run Sheet'!$D$2:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1631,7 +1690,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$E$1</c:f>
+              <c:f>'70 Run Sheet'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1666,7 +1725,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1723,7 +1782,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$E$2:$E$17</c:f>
+              <c:f>'70 Run Sheet'!$E$2:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1790,7 +1849,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$F$1</c:f>
+              <c:f>'70 Run Sheet'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1825,7 +1884,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1882,7 +1941,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$F$2:$F$17</c:f>
+              <c:f>'70 Run Sheet'!$F$2:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1901,7 +1960,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$G$1</c:f>
+              <c:f>'70 Run Sheet'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1936,7 +1995,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1993,7 +2052,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$G$2:$G$17</c:f>
+              <c:f>'70 Run Sheet'!$G$2:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2012,7 +2071,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$H$1</c:f>
+              <c:f>'70 Run Sheet'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2053,7 +2112,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2110,7 +2169,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$H$2:$H$17</c:f>
+              <c:f>'70 Run Sheet'!$H$2:$H$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2129,7 +2188,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$I$1</c:f>
+              <c:f>'70 Run Sheet'!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2170,7 +2229,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2227,7 +2286,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$I$2:$I$17</c:f>
+              <c:f>'70 Run Sheet'!$I$2:$I$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2246,7 +2305,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$J$1</c:f>
+              <c:f>'70 Run Sheet'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2287,7 +2346,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2344,7 +2403,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$J$2:$J$17</c:f>
+              <c:f>'70 Run Sheet'!$J$2:$J$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2363,7 +2422,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$K$1</c:f>
+              <c:f>'70 Run Sheet'!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2404,7 +2463,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2461,7 +2520,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$K$2:$K$17</c:f>
+              <c:f>'70 Run Sheet'!$K$2:$K$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2480,7 +2539,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$L$1</c:f>
+              <c:f>'70 Run Sheet'!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2521,7 +2580,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2578,7 +2637,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$L$2:$L$17</c:f>
+              <c:f>'70 Run Sheet'!$L$2:$L$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2597,7 +2656,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$M$1</c:f>
+              <c:f>'70 Run Sheet'!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2638,7 +2697,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2695,7 +2754,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$M$2:$M$17</c:f>
+              <c:f>'70 Run Sheet'!$M$2:$M$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2714,7 +2773,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$N$1</c:f>
+              <c:f>'70 Run Sheet'!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2758,7 +2817,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2815,7 +2874,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$N$2:$N$17</c:f>
+              <c:f>'70 Run Sheet'!$N$2:$N$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2834,7 +2893,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$O$1</c:f>
+              <c:f>'70 Run Sheet'!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2878,7 +2937,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2935,7 +2994,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$O$2:$O$17</c:f>
+              <c:f>'70 Run Sheet'!$O$2:$O$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2954,7 +3013,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$P$1</c:f>
+              <c:f>'70 Run Sheet'!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2998,7 +3057,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3055,7 +3114,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$P$2:$P$17</c:f>
+              <c:f>'70 Run Sheet'!$P$2:$P$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3074,7 +3133,7 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$Q$1</c:f>
+              <c:f>'70 Run Sheet'!$Q$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3118,7 +3177,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3175,7 +3234,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$Q$2:$Q$17</c:f>
+              <c:f>'70 Run Sheet'!$Q$2:$Q$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3194,7 +3253,7 @@
           <c:order val="16"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$R$1</c:f>
+              <c:f>'70 Run Sheet'!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3238,7 +3297,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3295,7 +3354,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$R$2:$R$17</c:f>
+              <c:f>'70 Run Sheet'!$R$2:$R$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3314,7 +3373,7 @@
           <c:order val="17"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$S$1</c:f>
+              <c:f>'70 Run Sheet'!$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3358,7 +3417,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3415,7 +3474,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$S$2:$S$17</c:f>
+              <c:f>'70 Run Sheet'!$S$2:$S$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3434,7 +3493,7 @@
           <c:order val="18"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$T$1</c:f>
+              <c:f>'70 Run Sheet'!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3475,7 +3534,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3532,7 +3591,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$T$2:$T$17</c:f>
+              <c:f>'70 Run Sheet'!$T$2:$T$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3551,7 +3610,7 @@
           <c:order val="19"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$U$1</c:f>
+              <c:f>'70 Run Sheet'!$U$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3592,7 +3651,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3649,7 +3708,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$U$2:$U$17</c:f>
+              <c:f>'70 Run Sheet'!$U$2:$U$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3668,7 +3727,7 @@
           <c:order val="20"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$V$1</c:f>
+              <c:f>'70 Run Sheet'!$V$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3709,7 +3768,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3766,7 +3825,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$V$2:$V$17</c:f>
+              <c:f>'70 Run Sheet'!$V$2:$V$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3785,7 +3844,7 @@
           <c:order val="21"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$W$1</c:f>
+              <c:f>'70 Run Sheet'!$W$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3826,7 +3885,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3883,7 +3942,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$W$2:$W$17</c:f>
+              <c:f>'70 Run Sheet'!$W$2:$W$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3902,7 +3961,7 @@
           <c:order val="22"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$X$1</c:f>
+              <c:f>'70 Run Sheet'!$X$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3943,7 +4002,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4000,7 +4059,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$X$2:$X$17</c:f>
+              <c:f>'70 Run Sheet'!$X$2:$X$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4019,7 +4078,7 @@
           <c:order val="23"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$Y$1</c:f>
+              <c:f>'70 Run Sheet'!$Y$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4060,7 +4119,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4117,7 +4176,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$Y$2:$Y$17</c:f>
+              <c:f>'70 Run Sheet'!$Y$2:$Y$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4136,7 +4195,7 @@
           <c:order val="24"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$Z$1</c:f>
+              <c:f>'70 Run Sheet'!$Z$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4180,7 +4239,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4237,7 +4296,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$Z$2:$Z$17</c:f>
+              <c:f>'70 Run Sheet'!$Z$2:$Z$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4256,7 +4315,7 @@
           <c:order val="25"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AA$1</c:f>
+              <c:f>'70 Run Sheet'!$AA$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4300,7 +4359,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4357,7 +4416,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AA$2:$AA$17</c:f>
+              <c:f>'70 Run Sheet'!$AA$2:$AA$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4376,7 +4435,7 @@
           <c:order val="26"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AB$1</c:f>
+              <c:f>'70 Run Sheet'!$AB$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4420,7 +4479,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4477,7 +4536,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AB$2:$AB$17</c:f>
+              <c:f>'70 Run Sheet'!$AB$2:$AB$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4496,7 +4555,7 @@
           <c:order val="27"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AC$1</c:f>
+              <c:f>'70 Run Sheet'!$AC$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4540,7 +4599,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4597,7 +4656,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AC$2:$AC$17</c:f>
+              <c:f>'70 Run Sheet'!$AC$2:$AC$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4616,7 +4675,7 @@
           <c:order val="28"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AD$1</c:f>
+              <c:f>'70 Run Sheet'!$AD$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4660,7 +4719,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4717,7 +4776,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AD$2:$AD$17</c:f>
+              <c:f>'70 Run Sheet'!$AD$2:$AD$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4736,7 +4795,7 @@
           <c:order val="29"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AE$1</c:f>
+              <c:f>'70 Run Sheet'!$AE$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4780,7 +4839,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4837,7 +4896,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AE$2:$AE$17</c:f>
+              <c:f>'70 Run Sheet'!$AE$2:$AE$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4856,7 +4915,7 @@
           <c:order val="30"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AF$1</c:f>
+              <c:f>'70 Run Sheet'!$AF$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4897,7 +4956,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4954,7 +5013,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AF$2:$AF$17</c:f>
+              <c:f>'70 Run Sheet'!$AF$2:$AF$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4973,7 +5032,7 @@
           <c:order val="31"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AG$1</c:f>
+              <c:f>'70 Run Sheet'!$AG$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5014,7 +5073,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5071,7 +5130,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AG$2:$AG$17</c:f>
+              <c:f>'70 Run Sheet'!$AG$2:$AG$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5090,7 +5149,7 @@
           <c:order val="32"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AH$1</c:f>
+              <c:f>'70 Run Sheet'!$AH$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5131,7 +5190,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5188,7 +5247,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AH$2:$AH$17</c:f>
+              <c:f>'70 Run Sheet'!$AH$2:$AH$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5207,7 +5266,7 @@
           <c:order val="33"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AI$1</c:f>
+              <c:f>'70 Run Sheet'!$AI$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5248,7 +5307,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5305,7 +5364,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AI$2:$AI$17</c:f>
+              <c:f>'70 Run Sheet'!$AI$2:$AI$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5324,7 +5383,7 @@
           <c:order val="34"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AJ$1</c:f>
+              <c:f>'70 Run Sheet'!$AJ$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5365,7 +5424,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5422,7 +5481,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AJ$2:$AJ$17</c:f>
+              <c:f>'70 Run Sheet'!$AJ$2:$AJ$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5441,7 +5500,7 @@
           <c:order val="35"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AK$1</c:f>
+              <c:f>'70 Run Sheet'!$AK$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5482,7 +5541,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5539,7 +5598,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AK$2:$AK$17</c:f>
+              <c:f>'70 Run Sheet'!$AK$2:$AK$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5558,7 +5617,7 @@
           <c:order val="36"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AL$1</c:f>
+              <c:f>'70 Run Sheet'!$AL$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5602,7 +5661,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5659,7 +5718,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AL$2:$AL$17</c:f>
+              <c:f>'70 Run Sheet'!$AL$2:$AL$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5678,7 +5737,7 @@
           <c:order val="37"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AM$1</c:f>
+              <c:f>'70 Run Sheet'!$AM$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5722,7 +5781,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5779,7 +5838,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AM$2:$AM$17</c:f>
+              <c:f>'70 Run Sheet'!$AM$2:$AM$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5798,7 +5857,7 @@
           <c:order val="38"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AN$1</c:f>
+              <c:f>'70 Run Sheet'!$AN$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5842,7 +5901,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5899,7 +5958,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AN$2:$AN$17</c:f>
+              <c:f>'70 Run Sheet'!$AN$2:$AN$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5918,7 +5977,7 @@
           <c:order val="39"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AO$1</c:f>
+              <c:f>'70 Run Sheet'!$AO$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5962,7 +6021,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6019,7 +6078,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AO$2:$AO$17</c:f>
+              <c:f>'70 Run Sheet'!$AO$2:$AO$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6038,7 +6097,7 @@
           <c:order val="40"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AP$1</c:f>
+              <c:f>'70 Run Sheet'!$AP$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6082,7 +6141,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6139,7 +6198,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AP$2:$AP$17</c:f>
+              <c:f>'70 Run Sheet'!$AP$2:$AP$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6158,7 +6217,7 @@
           <c:order val="41"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AQ$1</c:f>
+              <c:f>'70 Run Sheet'!$AQ$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6202,7 +6261,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6259,7 +6318,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AQ$2:$AQ$17</c:f>
+              <c:f>'70 Run Sheet'!$AQ$2:$AQ$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6278,7 +6337,7 @@
           <c:order val="42"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AR$1</c:f>
+              <c:f>'70 Run Sheet'!$AR$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6319,7 +6378,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6376,7 +6435,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AR$2:$AR$17</c:f>
+              <c:f>'70 Run Sheet'!$AR$2:$AR$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6395,7 +6454,7 @@
           <c:order val="43"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AS$1</c:f>
+              <c:f>'70 Run Sheet'!$AS$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6436,7 +6495,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6493,7 +6552,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AS$2:$AS$17</c:f>
+              <c:f>'70 Run Sheet'!$AS$2:$AS$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6512,7 +6571,7 @@
           <c:order val="44"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AT$1</c:f>
+              <c:f>'70 Run Sheet'!$AT$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6553,7 +6612,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6610,7 +6669,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AT$2:$AT$17</c:f>
+              <c:f>'70 Run Sheet'!$AT$2:$AT$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6629,7 +6688,7 @@
           <c:order val="45"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AU$1</c:f>
+              <c:f>'70 Run Sheet'!$AU$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6670,7 +6729,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6727,7 +6786,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AU$2:$AU$17</c:f>
+              <c:f>'70 Run Sheet'!$AU$2:$AU$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6746,7 +6805,7 @@
           <c:order val="46"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AV$1</c:f>
+              <c:f>'70 Run Sheet'!$AV$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6787,7 +6846,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6844,7 +6903,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AV$2:$AV$17</c:f>
+              <c:f>'70 Run Sheet'!$AV$2:$AV$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6863,7 +6922,7 @@
           <c:order val="47"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AW$1</c:f>
+              <c:f>'70 Run Sheet'!$AW$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6904,7 +6963,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6961,7 +7020,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AW$2:$AW$17</c:f>
+              <c:f>'70 Run Sheet'!$AW$2:$AW$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -6980,7 +7039,7 @@
           <c:order val="48"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AX$1</c:f>
+              <c:f>'70 Run Sheet'!$AX$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7024,7 +7083,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7081,7 +7140,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AX$2:$AX$17</c:f>
+              <c:f>'70 Run Sheet'!$AX$2:$AX$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7100,7 +7159,7 @@
           <c:order val="49"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AY$1</c:f>
+              <c:f>'70 Run Sheet'!$AY$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7144,7 +7203,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7201,7 +7260,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AY$2:$AY$17</c:f>
+              <c:f>'70 Run Sheet'!$AY$2:$AY$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7220,7 +7279,7 @@
           <c:order val="50"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$AZ$1</c:f>
+              <c:f>'70 Run Sheet'!$AZ$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7264,7 +7323,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7321,7 +7380,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$AZ$2:$AZ$17</c:f>
+              <c:f>'70 Run Sheet'!$AZ$2:$AZ$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7340,7 +7399,7 @@
           <c:order val="51"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BA$1</c:f>
+              <c:f>'70 Run Sheet'!$BA$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7384,7 +7443,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7441,7 +7500,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BA$2:$BA$17</c:f>
+              <c:f>'70 Run Sheet'!$BA$2:$BA$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7460,7 +7519,7 @@
           <c:order val="52"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BB$1</c:f>
+              <c:f>'70 Run Sheet'!$BB$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7504,7 +7563,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7561,7 +7620,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BB$2:$BB$17</c:f>
+              <c:f>'70 Run Sheet'!$BB$2:$BB$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7580,7 +7639,7 @@
           <c:order val="53"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BC$1</c:f>
+              <c:f>'70 Run Sheet'!$BC$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7624,7 +7683,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7681,7 +7740,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BC$2:$BC$17</c:f>
+              <c:f>'70 Run Sheet'!$BC$2:$BC$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7700,7 +7759,7 @@
           <c:order val="54"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BD$1</c:f>
+              <c:f>'70 Run Sheet'!$BD$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7735,7 +7794,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7792,7 +7851,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BD$2:$BD$17</c:f>
+              <c:f>'70 Run Sheet'!$BD$2:$BD$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7811,7 +7870,7 @@
           <c:order val="55"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BE$1</c:f>
+              <c:f>'70 Run Sheet'!$BE$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7846,7 +7905,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7903,7 +7962,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BE$2:$BE$17</c:f>
+              <c:f>'70 Run Sheet'!$BE$2:$BE$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7922,7 +7981,7 @@
           <c:order val="56"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BF$1</c:f>
+              <c:f>'70 Run Sheet'!$BF$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7957,7 +8016,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8014,7 +8073,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BF$2:$BF$17</c:f>
+              <c:f>'70 Run Sheet'!$BF$2:$BF$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8033,7 +8092,7 @@
           <c:order val="57"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BG$1</c:f>
+              <c:f>'70 Run Sheet'!$BG$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8068,7 +8127,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8125,7 +8184,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BG$2:$BG$17</c:f>
+              <c:f>'70 Run Sheet'!$BG$2:$BG$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8144,7 +8203,7 @@
           <c:order val="58"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BH$1</c:f>
+              <c:f>'70 Run Sheet'!$BH$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8179,7 +8238,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8236,7 +8295,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BH$2:$BH$17</c:f>
+              <c:f>'70 Run Sheet'!$BH$2:$BH$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8255,7 +8314,7 @@
           <c:order val="59"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BI$1</c:f>
+              <c:f>'70 Run Sheet'!$BI$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8290,7 +8349,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8347,7 +8406,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BI$2:$BI$17</c:f>
+              <c:f>'70 Run Sheet'!$BI$2:$BI$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8366,7 +8425,7 @@
           <c:order val="60"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BJ$1</c:f>
+              <c:f>'70 Run Sheet'!$BJ$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8407,7 +8466,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8464,7 +8523,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BJ$2:$BJ$17</c:f>
+              <c:f>'70 Run Sheet'!$BJ$2:$BJ$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8483,7 +8542,7 @@
           <c:order val="61"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BK$1</c:f>
+              <c:f>'70 Run Sheet'!$BK$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8524,7 +8583,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8581,7 +8640,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BK$2:$BK$17</c:f>
+              <c:f>'70 Run Sheet'!$BK$2:$BK$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8600,7 +8659,7 @@
           <c:order val="62"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BL$1</c:f>
+              <c:f>'70 Run Sheet'!$BL$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8641,7 +8700,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8698,7 +8757,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BL$2:$BL$17</c:f>
+              <c:f>'70 Run Sheet'!$BL$2:$BL$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8717,7 +8776,7 @@
           <c:order val="63"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BM$1</c:f>
+              <c:f>'70 Run Sheet'!$BM$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8758,7 +8817,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8815,7 +8874,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BM$2:$BM$17</c:f>
+              <c:f>'70 Run Sheet'!$BM$2:$BM$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8834,7 +8893,7 @@
           <c:order val="64"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BN$1</c:f>
+              <c:f>'70 Run Sheet'!$BN$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8875,7 +8934,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8932,7 +8991,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BN$2:$BN$17</c:f>
+              <c:f>'70 Run Sheet'!$BN$2:$BN$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8951,7 +9010,7 @@
           <c:order val="65"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BO$1</c:f>
+              <c:f>'70 Run Sheet'!$BO$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8992,7 +9051,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -9049,7 +9108,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BO$2:$BO$17</c:f>
+              <c:f>'70 Run Sheet'!$BO$2:$BO$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -9068,7 +9127,7 @@
           <c:order val="66"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BP$1</c:f>
+              <c:f>'70 Run Sheet'!$BP$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9112,7 +9171,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -9169,7 +9228,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BP$2:$BP$17</c:f>
+              <c:f>'70 Run Sheet'!$BP$2:$BP$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -9188,7 +9247,7 @@
           <c:order val="67"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BQ$1</c:f>
+              <c:f>'70 Run Sheet'!$BQ$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9232,7 +9291,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -9289,7 +9348,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BQ$2:$BQ$17</c:f>
+              <c:f>'70 Run Sheet'!$BQ$2:$BQ$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -9308,7 +9367,7 @@
           <c:order val="68"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BR$1</c:f>
+              <c:f>'70 Run Sheet'!$BR$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9352,7 +9411,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -9409,7 +9468,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BR$2:$BR$17</c:f>
+              <c:f>'70 Run Sheet'!$BR$2:$BR$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -9428,7 +9487,7 @@
           <c:order val="69"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$BS$1</c:f>
+              <c:f>'70 Run Sheet'!$BS$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9472,7 +9531,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$2:$A$17</c:f>
+              <c:f>'70 Run Sheet'!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -9529,7 +9588,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$BS$2:$BS$17</c:f>
+              <c:f>'70 Run Sheet'!$BS$2:$BS$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -9582,7 +9641,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -9614,7 +9673,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -9652,7 +9711,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -9700,7 +9759,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -9732,7 +9791,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -9770,7 +9829,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -9828,7 +9887,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1400"/>
+        <a:defRPr sz="1800"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -10952,7 +11011,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C19AB7F7-4B36-4B7A-A5C6-55656F7565F0}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
@@ -11039,21 +11098,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B07C8A63-BE9A-4035-8D9A-ED7C76885D03}" name="Table1" displayName="Table1" ref="A1:G17" totalsRowShown="0">
-  <autoFilter ref="A1:G17" xr:uid="{B07C8A63-BE9A-4035-8D9A-ED7C76885D03}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B07C8A63-BE9A-4035-8D9A-ED7C76885D03}" name="Table1" displayName="Table1" ref="A1:H17" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:H17" xr:uid="{B07C8A63-BE9A-4035-8D9A-ED7C76885D03}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{827C73A7-58F1-4703-8AB7-40D9E026E511}" name="Dec"/>
-    <tableColumn id="2" xr3:uid="{10D6A431-187E-4E90-BC95-C69DD5D4030E}" name="Hex" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{10D6A431-187E-4E90-BC95-C69DD5D4030E}" name="Hex" dataDxfId="5">
       <calculatedColumnFormula>DEC2HEX(Table1[[#This Row],[Dec]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8115C6CD-52D0-4D93-B3D3-01EB0D481935}" name="Unicode.java 20-Run Peformance Test (Avg. Time)" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{CFC26FED-0121-45CA-956E-A34C0146D063}" name="Unicode.java 70-Run Peformance Test (Avg. Time)" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{ACABCCCA-AACB-40CE-BB16-F1918F432D89}" name="New Implementation" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{E220D3B2-C7E8-4771-98D9-625541509279}" name="Improvement" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{8115C6CD-52D0-4D93-B3D3-01EB0D481935}" name="Unicode.java 20-Run Peformance Test (Avg. Time)" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CFC26FED-0121-45CA-956E-A34C0146D063}" name="Unicode.java 70-Run Peformance Test (Avg. Time)" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{ACABCCCA-AACB-40CE-BB16-F1918F432D89}" name="New Implementation" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{E220D3B2-C7E8-4771-98D9-625541509279}" name="Improvement" dataDxfId="1">
       <calculatedColumnFormula>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{8E7A133F-1CAF-4B76-9F3A-DFA09C49FB4A}" name="Fast/Slow">
       <calculatedColumnFormula>IF(F2&gt;0,"Faster","Slower")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{8BFF4E76-5F68-41CC-970C-508B2A13F98A}" name="Concatenated" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -11357,46 +11419,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630D28D3-0FC1-4AE2-AEF6-7064C7C9D076}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="47" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -11421,12 +11494,15 @@
         <f>IF(F2&gt;0,"Faster","Slower")</f>
         <v>Faster</v>
       </c>
-      <c r="I2" t="str">
-        <f t="shared" ref="I2:I17" si="0">_xlfn.CONCAT("0,",B2)</f>
+      <c r="H2" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,0</v>
       </c>
+      <c r="J2" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -11448,15 +11524,15 @@
         <v>5.0000000000000009E-5</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G17" si="1">IF(F3&gt;0,"Faster","Slower")</f>
+        <f t="shared" ref="G3:G17" si="0">IF(F3&gt;0,"Faster","Slower")</f>
         <v>Faster</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H3" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,A</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3*5</f>
         <v>50</v>
@@ -11479,15 +11555,15 @@
         <v>9.9999999999999991E-5</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
+      <c r="H4" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,32</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4*2</f>
         <v>100</v>
@@ -11510,15 +11586,15 @@
         <v>9.9999999999999991E-5</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
+      <c r="H5" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,64</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5*5</f>
         <v>500</v>
@@ -11541,15 +11617,15 @@
         <v>5.0000000000000023E-4</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
+      <c r="H6" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,1F4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6*2</f>
         <v>1000</v>
@@ -11572,15 +11648,15 @@
         <v>7.499999999999998E-4</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
+      <c r="H7" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,3E8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>A7*5</f>
         <v>5000</v>
@@ -11603,15 +11679,15 @@
         <v>2.0500000000000032E-3</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H8" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,1388</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>A8*2</f>
         <v>10000</v>
@@ -11634,15 +11710,15 @@
         <v>2.4500000000000043E-3</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
+      <c r="H9" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,2710</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A9*5</f>
         <v>50000</v>
@@ -11665,15 +11741,15 @@
         <v>6.4000000000000029E-3</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
+      <c r="H10" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,C350</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10*2</f>
         <v>100000</v>
@@ -11696,15 +11772,15 @@
         <v>9.7499999999999948E-3</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
+      <c r="H11" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,186A0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>A11*5</f>
         <v>500000</v>
@@ -11727,15 +11803,15 @@
         <v>5.325000000000002E-2</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
+      <c r="H12" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,7A120</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>A12*2</f>
         <v>1000000</v>
@@ -11758,15 +11834,15 @@
         <v>0.11150000000000038</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I13" t="str">
-        <f t="shared" si="0"/>
+      <c r="H13" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,F4240</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>A13*5</f>
         <v>5000000</v>
@@ -11789,15 +11865,15 @@
         <v>0.26774999999999904</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I14" t="str">
-        <f t="shared" si="0"/>
+      <c r="H14" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,4C4B40</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>A14*2</f>
         <v>10000000</v>
@@ -11820,15 +11896,15 @@
         <v>0.23735000000000106</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I15" t="str">
-        <f t="shared" si="0"/>
+      <c r="H15" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,989680</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>A15+(A15/2)</f>
         <v>15000000</v>
@@ -11851,15 +11927,15 @@
         <v>9.8900000000002208E-2</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I16" t="str">
-        <f t="shared" si="0"/>
+      <c r="H16" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,E4E1C0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17825791</v>
       </c>
@@ -11881,23 +11957,24 @@
         <v>8.8399999999996481E-2</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Faster</v>
       </c>
-      <c r="I17" t="str">
-        <f t="shared" si="0"/>
+      <c r="H17" t="str">
+        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,10FFFFF</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -11907,7 +11984,7 @@
   <dimension ref="A1:BT17"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E17"/>
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13638,15 +13715,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DA56391-5E7B-4534-8A0E-1586A9147009}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="80976a04-0ce1-4677-8b1b-aa81255844cf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="80976a04-0ce1-4677-8b1b-aa81255844cf"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Peformance improvement under works
</commit_message>
<xml_diff>
--- a/Simulation/CSARCH2 Proj Diagnostics.xlsx
+++ b/Simulation/CSARCH2 Proj Diagnostics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Miguel Escalona\Github\CSARCH2_Project\Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E86E320-77E8-4C1E-92BC-067C244FD87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334BFD2E-F948-4D34-97A8-E04FD7A54F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{E5B5E468-C3F2-49F0-9D6C-48D86FBE0D23}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Hex</t>
   </si>
@@ -58,15 +58,6 @@
     <t>Unicode.java 20-Run Peformance Test (Avg. Time)</t>
   </si>
   <si>
-    <t>Improvement</t>
-  </si>
-  <si>
-    <t>Fast/Slow</t>
-  </si>
-  <si>
-    <t>New Implementation</t>
-  </si>
-  <si>
     <t>Implementation</t>
   </si>
   <si>
@@ -76,13 +67,28 @@
     <t>Concatenated</t>
   </si>
   <si>
-    <t>Improvement2</t>
+    <t>New Implementation (Java, 20-Run)</t>
+  </si>
+  <si>
+    <t>JS Improvement</t>
+  </si>
+  <si>
+    <t>Java Improvement</t>
+  </si>
+  <si>
+    <t>Initial JS Version (1 Run)</t>
+  </si>
+  <si>
+    <t>JS Optimized New Implementation (1 Run)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -165,12 +171,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -181,18 +228,39 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -207,6 +275,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -215,6 +284,10 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -223,6 +296,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -238,6 +312,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -438,7 +517,7 @@
             <c:numRef>
               <c:f>Main_Sheet!$C$2:$C$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>8.0000000000000004E-4</c:v>
@@ -499,15 +578,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Main_Sheet!$D$1</c:f>
+              <c:f>Main_Sheet!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Unicode.java 70-Run Peformance Test (Avg. Time)</c:v>
+                  <c:v>New Implementation (Java, 20-Run)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -515,7 +594,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -526,166 +605,7 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Main_Sheet!$A$2:$A$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>50000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>10000000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15000000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>17825791</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Main_Sheet!$D$2:$D$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>3.5714285714285714E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.7142857142857142E-5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5714285714285719E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.2857142857142862E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.1428571428571492E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.4857142857142866E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.1285714285714329E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.4857142857142864E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.8671428571428564E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.15835714285714292</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.83719999999999983</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.6912714285714292</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.1687000000000003</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8.1156857142857159</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>11.641885714285715</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>13.069185714285714</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-ADDB-46EE-8839-E2938B320EF7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Main_Sheet!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>New Implementation</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
@@ -756,7 +676,7 @@
             <c:numRef>
               <c:f>Main_Sheet!$E$2:$E$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>6.0000000000000006E-4</c:v>
@@ -826,6 +746,338 @@
         </c:dLbls>
         <c:axId val="1702969584"/>
         <c:axId val="1702970000"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main_Sheet!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Initial JS Version (1 Run)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Main_Sheet!$A$2:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15000000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17825791</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Main_Sheet!$F$2:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0000000000000001E-18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.9999999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.252</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.60699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7040000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.4889999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29.077000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51.204000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>73.551000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>89.703000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BFC8-4852-8918-E4132DFB4576}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main_Sheet!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JS Optimized New Implementation (1 Run)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Main_Sheet!$A$2:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15000000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17825791</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Main_Sheet!$G$2:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.32800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.54100000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.145</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.383</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.352</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.582999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24.742000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31.718</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-BFC8-4852-8918-E4132DFB4576}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2005578943"/>
+        <c:axId val="1940225791"/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="1702969584"/>
@@ -986,7 +1238,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-PH"/>
-                  <a:t>Time Taken (seconds)</a:t>
+                  <a:t>Java Time Taken (seconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1020,7 +1272,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1061,9 +1313,38 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="1940225791"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2005578943"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2005578943"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1940225791"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -1072,7 +1353,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:legendEntry>
-        <c:idx val="3"/>
+        <c:idx val="4"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:overlay val="0"/>
@@ -11021,7 +11302,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C19AB7F7-4B36-4B7A-A5C6-55656F7565F0}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="87" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
@@ -11033,7 +11314,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E27F99DC-DCFC-40B0-8C2B-48C8420F506E}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="87" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
@@ -11045,7 +11326,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="11404934" cy="6291513"/>
+    <xdr:ext cx="11419052" cy="6295259"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11078,7 +11359,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="11404934" cy="6291513"/>
+    <xdr:ext cx="11419052" cy="6295259"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11108,27 +11389,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B07C8A63-BE9A-4035-8D9A-ED7C76885D03}" name="Table1" displayName="Table1" ref="A1:I17" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B07C8A63-BE9A-4035-8D9A-ED7C76885D03}" name="Table1" displayName="Table1" ref="A1:I17" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:I17" xr:uid="{B07C8A63-BE9A-4035-8D9A-ED7C76885D03}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{827C73A7-58F1-4703-8AB7-40D9E026E511}" name="Dec"/>
-    <tableColumn id="2" xr3:uid="{10D6A431-187E-4E90-BC95-C69DD5D4030E}" name="Hex" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{10D6A431-187E-4E90-BC95-C69DD5D4030E}" name="Hex" dataDxfId="6">
       <calculatedColumnFormula>DEC2HEX(Table1[[#This Row],[Dec]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8115C6CD-52D0-4D93-B3D3-01EB0D481935}" name="Unicode.java 20-Run Peformance Test (Avg. Time)" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{CFC26FED-0121-45CA-956E-A34C0146D063}" name="Unicode.java 70-Run Peformance Test (Avg. Time)" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{ACABCCCA-AACB-40CE-BB16-F1918F432D89}" name="New Implementation" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{E220D3B2-C7E8-4771-98D9-625541509279}" name="Improvement" dataDxfId="0">
-      <calculatedColumnFormula>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{8115C6CD-52D0-4D93-B3D3-01EB0D481935}" name="Unicode.java 20-Run Peformance Test (Avg. Time)" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{CFC26FED-0121-45CA-956E-A34C0146D063}" name="Unicode.java 70-Run Peformance Test (Avg. Time)" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{ACABCCCA-AACB-40CE-BB16-F1918F432D89}" name="New Implementation (Java, 20-Run)" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{5E6692CA-DF37-46CC-8395-0F19AECE18BA}" name="Initial JS Version (1 Run)" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{BA56667D-2969-4F79-B363-777216C985A4}" name="JS Optimized New Implementation (1 Run)" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{8E7A133F-1CAF-4B76-9F3A-DFA09C49FB4A}" name="Java Improvement">
+      <calculatedColumnFormula>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{8E7A133F-1CAF-4B76-9F3A-DFA09C49FB4A}" name="Fast/Slow">
-      <calculatedColumnFormula>IF(F2&gt;0,"Faster","Slower")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{8BFF4E76-5F68-41CC-970C-508B2A13F98A}" name="Improvement2" dataCellStyle="Percent">
-      <calculatedColumnFormula>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{3DDFC604-B960-4571-887B-E2B5CD0294ED}" name="Concatenated">
-      <calculatedColumnFormula>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{8BFF4E76-5F68-41CC-970C-508B2A13F98A}" name="JS Improvement" dataDxfId="3" dataCellStyle="Percent">
+      <calculatedColumnFormula>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -11432,10 +11709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630D28D3-0FC1-4AE2-AEF6-7064C7C9D076}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11445,15 +11722,14 @@
     <col min="3" max="3" width="26" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -11467,25 +11743,28 @@
         <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="K1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -11493,36 +11772,38 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="7">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="7">
         <v>3.5714285714285714E-4</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="7">
         <v>6.0000000000000006E-4</v>
       </c>
-      <c r="F2">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>1.9999999999999998E-4</v>
-      </c>
-      <c r="G2" t="str">
-        <f>IF(F2&gt;0,"Faster","Slower")</f>
-        <v>Faster</v>
-      </c>
-      <c r="H2" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+      <c r="F2" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
         <v>0.24999999999999997</v>
       </c>
-      <c r="I2" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
+      <c r="I2" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="11" t="str">
+        <f>_xlfn.CONCAT("0,",B2)</f>
         <v>0,0</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>10</v>
+      <c r="K2" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -11530,33 +11811,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>A</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="7">
         <v>1.5000000000000001E-4</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="7">
         <v>5.7142857142857142E-5</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="7">
         <v>1E-4</v>
       </c>
-      <c r="F3">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>5.0000000000000009E-5</v>
-      </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G17" si="0">IF(F3&gt;0,"Faster","Slower")</f>
-        <v>Faster</v>
-      </c>
-      <c r="H3" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+      <c r="F3" s="7">
+        <v>1.0000000000000001E-18</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
         <v>0.33333333333333337</v>
       </c>
-      <c r="I3" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
+      <c r="I3" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="11" t="str">
+        <f t="shared" ref="J3:J17" si="0">_xlfn.CONCAT("0,",B3)</f>
         <v>0,A</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3*5</f>
         <v>50</v>
@@ -11565,33 +11848,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>32</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="7">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="7">
         <v>1.5714285714285719E-4</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="7">
         <v>1.5000000000000001E-4</v>
       </c>
-      <c r="F4">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>9.9999999999999991E-5</v>
-      </c>
-      <c r="G4" t="str">
+      <c r="F4" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="H4">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="I4" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H4" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>0.39999999999999997</v>
-      </c>
-      <c r="I4" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4*2</f>
         <v>100</v>
@@ -11600,33 +11885,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>64</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="7">
         <v>3.5E-4</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="7">
         <v>2.2857142857142862E-4</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="7">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="F5">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>9.9999999999999991E-5</v>
-      </c>
-      <c r="G5" t="str">
+      <c r="F5" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="H5">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="I5" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H5" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="I5" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,64</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5*5</f>
         <v>500</v>
@@ -11635,33 +11922,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>1F4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="7">
         <v>1.4500000000000006E-3</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="7">
         <v>9.1428571428571492E-4</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="7">
         <v>9.5000000000000032E-4</v>
       </c>
-      <c r="F6">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>5.0000000000000023E-4</v>
-      </c>
-      <c r="G6" t="str">
+      <c r="F6" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="G6" s="7">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H6">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>0.34482758620689657</v>
+      </c>
+      <c r="I6" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>0.2</v>
+      </c>
+      <c r="J6" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H6" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>0.34482758620689657</v>
-      </c>
-      <c r="I6" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,1F4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6*2</f>
         <v>1000</v>
@@ -11670,33 +11959,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>3E8</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="7">
         <v>2.0500000000000006E-3</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="7">
         <v>1.4857142857142866E-3</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="7">
         <v>1.3000000000000008E-3</v>
       </c>
-      <c r="F7">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>7.499999999999998E-4</v>
-      </c>
-      <c r="G7" t="str">
+      <c r="F7" s="7">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1.2E-2</v>
+      </c>
+      <c r="H7">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>0.36585365853658514</v>
+      </c>
+      <c r="I7" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>-0.33333333333333348</v>
+      </c>
+      <c r="J7" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H7" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>0.36585365853658514</v>
-      </c>
-      <c r="I7" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,3E8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>A7*5</f>
         <v>5000</v>
@@ -11705,33 +11996,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>1388</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="7">
         <v>8.0500000000000051E-3</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="7">
         <v>7.1285714285714329E-3</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="7">
         <v>6.0000000000000019E-3</v>
       </c>
-      <c r="F8">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>2.0500000000000032E-3</v>
-      </c>
-      <c r="G8" t="str">
+      <c r="F8" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G8" s="7">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="H8">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>0.25465838509316796</v>
+      </c>
+      <c r="I8" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>-8.8888888888888976E-2</v>
+      </c>
+      <c r="J8" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H8" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>0.25465838509316796</v>
-      </c>
-      <c r="I8" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,1388</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>A8*2</f>
         <v>10000</v>
@@ -11740,33 +12033,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>2710</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="7">
         <v>1.4050000000000007E-2</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="7">
         <v>1.4857142857142864E-2</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="7">
         <v>1.1600000000000003E-2</v>
       </c>
-      <c r="F9">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>2.4500000000000043E-3</v>
-      </c>
-      <c r="G9" t="str">
+      <c r="F9" s="7">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="G9" s="7">
+        <v>6.3E-2</v>
+      </c>
+      <c r="H9">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>0.17437722419928847</v>
+      </c>
+      <c r="I9" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>-0.18867924528301891</v>
+      </c>
+      <c r="J9" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H9" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>0.17437722419928847</v>
-      </c>
-      <c r="I9" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,2710</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A9*5</f>
         <v>50000</v>
@@ -11775,33 +12070,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>C350</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="7">
         <v>5.7450000000000022E-2</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="7">
         <v>6.8671428571428564E-2</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="7">
         <v>5.1050000000000019E-2</v>
       </c>
-      <c r="F10">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>6.4000000000000029E-3</v>
-      </c>
-      <c r="G10" t="str">
+      <c r="F10" s="7">
+        <v>0.252</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="H10">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>0.11140121845082682</v>
+      </c>
+      <c r="I10" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>-0.30158730158730163</v>
+      </c>
+      <c r="J10" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H10" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>0.11140121845082682</v>
-      </c>
-      <c r="I10" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,C350</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10*2</f>
         <v>100000</v>
@@ -11810,33 +12107,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>186A0</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="7">
         <v>0.1203</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="7">
         <v>0.15835714285714292</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="7">
         <v>0.11055000000000001</v>
       </c>
-      <c r="F11">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>9.7499999999999948E-3</v>
-      </c>
-      <c r="G11" t="str">
+      <c r="F11" s="7">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="H11">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>8.1047381546134611E-2</v>
+      </c>
+      <c r="I11" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>0.10873146622734753</v>
+      </c>
+      <c r="J11" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H11" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>8.1047381546134611E-2</v>
-      </c>
-      <c r="I11" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,186A0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>A11*5</f>
         <v>500000</v>
@@ -11845,33 +12144,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>7A120</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="7">
         <v>0.65759999999999996</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="7">
         <v>0.83719999999999983</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="7">
         <v>0.60434999999999994</v>
       </c>
-      <c r="F12">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>5.325000000000002E-2</v>
-      </c>
-      <c r="G12" t="str">
+      <c r="F12" s="7">
+        <v>3.7040000000000002</v>
+      </c>
+      <c r="G12" s="7">
+        <v>2.145</v>
+      </c>
+      <c r="H12">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>8.0976277372262803E-2</v>
+      </c>
+      <c r="I12" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>0.42089632829373652</v>
+      </c>
+      <c r="J12" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H12" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>8.0976277372262803E-2</v>
-      </c>
-      <c r="I12" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,7A120</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>A12*2</f>
         <v>1000000</v>
@@ -11880,33 +12181,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>F4240</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="7">
         <v>1.3039000000000001</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="7">
         <v>1.6912714285714292</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="7">
         <v>1.1923999999999997</v>
       </c>
-      <c r="F13">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>0.11150000000000038</v>
-      </c>
-      <c r="G13" t="str">
+      <c r="F13" s="7">
+        <v>7.4889999999999999</v>
+      </c>
+      <c r="G13" s="7">
+        <v>4.383</v>
+      </c>
+      <c r="H13">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>8.5512692691157577E-2</v>
+      </c>
+      <c r="I13" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>0.41474162104419815</v>
+      </c>
+      <c r="J13" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H13" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>8.5512692691157577E-2</v>
-      </c>
-      <c r="I13" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,F4240</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>A13*5</f>
         <v>5000000</v>
@@ -11915,33 +12218,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>4C4B40</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="7">
         <v>4.0007999999999999</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="7">
         <v>5.1687000000000003</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="7">
         <v>3.7330500000000009</v>
       </c>
-      <c r="F14">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>0.26774999999999904</v>
-      </c>
-      <c r="G14" t="str">
+      <c r="F14" s="7">
+        <v>29.077000000000002</v>
+      </c>
+      <c r="G14" s="7">
+        <v>12.352</v>
+      </c>
+      <c r="H14">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>6.6924115176964366E-2</v>
+      </c>
+      <c r="I14" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>0.5751968910135159</v>
+      </c>
+      <c r="J14" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H14" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>6.6924115176964366E-2</v>
-      </c>
-      <c r="I14" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,4C4B40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>A14*2</f>
         <v>10000000</v>
@@ -11950,33 +12255,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>989680</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="7">
         <v>6.2537000000000011</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="7">
         <v>8.1156857142857159</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="7">
         <v>6.0163500000000001</v>
       </c>
-      <c r="F15">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>0.23735000000000106</v>
-      </c>
-      <c r="G15" t="str">
+      <c r="F15" s="7">
+        <v>51.204000000000001</v>
+      </c>
+      <c r="G15" s="7">
+        <v>18.582999999999998</v>
+      </c>
+      <c r="H15">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>3.7953531509346626E-2</v>
+      </c>
+      <c r="I15" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>0.63707913444262165</v>
+      </c>
+      <c r="J15" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H15" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>3.7953531509346626E-2</v>
-      </c>
-      <c r="I15" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,989680</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>A15+(A15/2)</f>
         <v>15000000</v>
@@ -11985,33 +12292,35 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>E4E1C0</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="7">
         <v>8.3956000000000017</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="7">
         <v>11.641885714285715</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="7">
         <v>8.2966999999999995</v>
       </c>
-      <c r="F16">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>9.8900000000002208E-2</v>
-      </c>
-      <c r="G16" t="str">
+      <c r="F16" s="7">
+        <v>73.551000000000002</v>
+      </c>
+      <c r="G16" s="7">
+        <v>24.742000000000001</v>
+      </c>
+      <c r="H16">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>1.1779979989518579E-2</v>
+      </c>
+      <c r="I16" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>0.6636075648189691</v>
+      </c>
+      <c r="J16" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H16" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>1.1779979989518579E-2</v>
-      </c>
-      <c r="I16" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,E4E1C0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17825791</v>
       </c>
@@ -12019,35 +12328,43 @@
         <f>DEC2HEX(Table1[[#This Row],[Dec]])</f>
         <v>10FFFFF</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="7">
         <v>9.6625999999999976</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="7">
         <v>13.069185714285714</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="7">
         <v>9.5742000000000012</v>
       </c>
-      <c r="F17">
-        <f>Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation]]</f>
-        <v>8.8399999999996481E-2</v>
-      </c>
-      <c r="G17" t="str">
+      <c r="F17" s="7">
+        <v>89.703000000000003</v>
+      </c>
+      <c r="G17" s="7">
+        <v>31.718</v>
+      </c>
+      <c r="H17">
+        <f>(Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]-Table1[[#This Row],[New Implementation (Java, 20-Run)]])/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
+        <v>9.1486763397011679E-3</v>
+      </c>
+      <c r="I17" s="6">
+        <f>(Table1[[#This Row],[Initial JS Version (1 Run)]]-Table1[[#This Row],[JS Optimized New Implementation (1 Run)]])/Table1[[#This Row],[Initial JS Version (1 Run)]]</f>
+        <v>0.64641093385951409</v>
+      </c>
+      <c r="J17" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>Faster</v>
-      </c>
-      <c r="H17" s="7">
-        <f>Table1[[#This Row],[Improvement]]/Table1[[#This Row],[Unicode.java 20-Run Peformance Test (Avg. Time)]]</f>
-        <v>9.1486763397011679E-3</v>
-      </c>
-      <c r="I17" t="str">
-        <f>_xlfn.CONCAT("0,",Table1[[#This Row],[Hex]])</f>
         <v>0,10FFFFF</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f>AVERAGE(Table1[JS Improvement])</f>
+        <v>0.29713594816296007</v>
       </c>
     </row>
   </sheetData>
@@ -13606,18 +13923,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13767,6 +14084,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CB5F086-3D4B-41EE-AD49-AC0E4F9160D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DA56391-5E7B-4534-8A0E-1586A9147009}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -13778,14 +14103,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CB5F086-3D4B-41EE-AD49-AC0E4F9160D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>